<commit_message>
Arnold MAXtoA Scripted Controller Files
</commit_message>
<xml_diff>
--- a/lens_shader_parameters_list.xlsx
+++ b/lens_shader_parameters_list.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="121">
   <si>
     <t>Mental ray</t>
   </si>
@@ -42,6 +42,9 @@
     <t>Max ID: 0x5b6d4650, 0x21e1666f</t>
   </si>
   <si>
+    <t>Max ID: 515151, 676100</t>
+  </si>
+  <si>
     <t>Latlong Stereo</t>
   </si>
   <si>
@@ -222,6 +225,9 @@
     <t>Max ID: 0x511a5e3e, 0x61393d01</t>
   </si>
   <si>
+    <t>Max ID: 515151, 676101</t>
+  </si>
+  <si>
     <t>domeAFL_FOV_Stereo</t>
   </si>
   <si>
@@ -343,6 +349,9 @@
   </si>
   <si>
     <t>domeAFL_WxH</t>
+  </si>
+  <si>
+    <t>Max ID: 515151, 676102</t>
   </si>
   <si>
     <t>DomemasterWxH</t>
@@ -395,7 +404,7 @@
     <font>
       <b val="1"/>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -420,7 +429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -435,16 +444,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -454,14 +463,14 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -477,9 +486,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -508,9 +514,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="fffa7d00"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff7f7f7f"/>
     </indexedColors>
   </colors>
@@ -662,9 +668,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -744,7 +750,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -772,10 +778,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1031,9 +1037,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1321,7 +1327,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1349,10 +1355,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1667,7 +1673,9 @@
       <c r="C5" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" t="s" s="4">
+        <v>9</v>
+      </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -1679,41 +1687,41 @@
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" t="s" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" t="s" s="7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s" s="7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s" s="7">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1721,38 +1729,38 @@
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" t="s" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1760,160 +1768,160 @@
     <row r="13" ht="15" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" t="s" s="7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" t="s" s="7">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s" s="7">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" t="s" s="7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s" s="7">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s" s="7">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s" s="7">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" t="s" s="7">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s" s="7">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s" s="7">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s" s="7">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s" s="8">
         <v>42</v>
       </c>
+      <c r="C18" t="s" s="7">
+        <v>43</v>
+      </c>
       <c r="D18" t="s" s="7">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" t="s" s="8">
-        <v>44</v>
+      <c r="C19" t="s" s="7">
+        <v>45</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" ht="15" customHeight="1">
       <c r="A20" s="2"/>
-      <c r="B20" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s" s="8">
+      <c r="B20" t="s" s="8">
         <v>46</v>
       </c>
-      <c r="D20" t="s" s="9">
+      <c r="C20" t="s" s="7">
         <v>47</v>
+      </c>
+      <c r="D20" t="s" s="8">
+        <v>48</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="A21" s="2"/>
-      <c r="B21" t="s" s="9">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s" s="8">
+      <c r="B21" t="s" s="8">
         <v>49</v>
       </c>
-      <c r="D21" t="s" s="9">
+      <c r="C21" t="s" s="7">
         <v>50</v>
+      </c>
+      <c r="D21" t="s" s="8">
+        <v>51</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="A22" s="2"/>
-      <c r="B22" t="s" s="9">
-        <v>51</v>
-      </c>
-      <c r="C22" t="s" s="8">
+      <c r="B22" t="s" s="8">
         <v>52</v>
       </c>
-      <c r="D22" t="s" s="9">
+      <c r="C22" t="s" s="7">
         <v>53</v>
+      </c>
+      <c r="D22" t="s" s="8">
+        <v>54</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="A23" s="2"/>
-      <c r="B23" t="s" s="9">
-        <v>54</v>
-      </c>
-      <c r="C23" t="s" s="8">
+      <c r="B23" t="s" s="8">
         <v>55</v>
       </c>
-      <c r="D23" t="s" s="9">
+      <c r="C23" t="s" s="7">
         <v>56</v>
+      </c>
+      <c r="D23" t="s" s="8">
+        <v>57</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" ht="15" customHeight="1">
       <c r="A24" s="2"/>
-      <c r="B24" t="s" s="9">
-        <v>57</v>
+      <c r="B24" t="s" s="8">
+        <v>58</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" t="s" s="9">
-        <v>58</v>
+      <c r="D24" t="s" s="8">
+        <v>59</v>
       </c>
       <c r="E24" s="2"/>
     </row>
@@ -1921,8 +1929,8 @@
       <c r="A25" s="2"/>
       <c r="B25" s="6"/>
       <c r="C25" s="2"/>
-      <c r="D25" t="s" s="9">
-        <v>59</v>
+      <c r="D25" t="s" s="8">
+        <v>60</v>
       </c>
       <c r="E25" s="2"/>
     </row>
@@ -1930,8 +1938,8 @@
       <c r="A26" s="2"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
-      <c r="D26" t="s" s="9">
-        <v>60</v>
+      <c r="D26" t="s" s="8">
+        <v>61</v>
       </c>
       <c r="E26" s="2"/>
     </row>
@@ -1939,8 +1947,8 @@
       <c r="A27" s="2"/>
       <c r="B27" s="6"/>
       <c r="C27" s="2"/>
-      <c r="D27" t="s" s="9">
-        <v>61</v>
+      <c r="D27" t="s" s="8">
+        <v>62</v>
       </c>
       <c r="E27" s="2"/>
     </row>
@@ -1948,8 +1956,8 @@
       <c r="A28" s="2"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
-      <c r="D28" t="s" s="9">
-        <v>62</v>
+      <c r="D28" t="s" s="8">
+        <v>63</v>
       </c>
       <c r="E28" s="2"/>
     </row>
@@ -1957,8 +1965,8 @@
       <c r="A29" s="2"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
-      <c r="D29" t="s" s="9">
-        <v>63</v>
+      <c r="D29" t="s" s="8">
+        <v>64</v>
       </c>
       <c r="E29" s="2"/>
     </row>
@@ -2000,25 +2008,27 @@
     <row r="35" ht="15" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" t="s" s="4">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s" s="4">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E35" t="s" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" t="s" s="4">
-        <v>68</v>
-      </c>
-      <c r="D36" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D36" t="s" s="4">
+        <v>70</v>
+      </c>
       <c r="E36" s="5"/>
     </row>
     <row r="37" ht="15" customHeight="1">
@@ -2030,58 +2040,58 @@
     </row>
     <row r="38" ht="15" customHeight="1">
       <c r="A38" t="s" s="4">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E38" t="s" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1">
       <c r="A39" t="s" s="4">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s" s="7">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s" s="7">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D39" t="s" s="7">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E39" t="s" s="7">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1">
       <c r="A40" s="2"/>
       <c r="B40" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D40" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E40" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2089,141 +2099,141 @@
     <row r="42" ht="15" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C42" t="s" s="7">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D42" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E42" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" t="s" s="7">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s" s="7">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s" s="7">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E43" t="s" s="7">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" t="s" s="7">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C44" t="s" s="7">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D44" t="s" s="7">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E44" t="s" s="7">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" t="s" s="7">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D45" t="s" s="7">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s" s="7">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" t="s" s="7">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s" s="7">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D46" t="s" s="7">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E46" t="s" s="7">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" t="s" s="7">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s" s="7">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D47" t="s" s="7">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E47" t="s" s="7">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" t="s" s="7">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D48" t="s" s="7">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E48" t="s" s="7">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="A49" s="2"/>
       <c r="B49" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C49" t="s" s="7">
         <v>35</v>
       </c>
-      <c r="C49" t="s" s="7">
-        <v>34</v>
-      </c>
       <c r="D49" t="s" s="7">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E49" s="2"/>
     </row>
     <row r="50" ht="15" customHeight="1">
       <c r="A50" s="2"/>
       <c r="B50" t="s" s="7">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s" s="7">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D50" t="s" s="7">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E50" s="2"/>
     </row>
     <row r="51" ht="15" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" t="s" s="7">
-        <v>93</v>
-      </c>
-      <c r="C51" t="s" s="8">
-        <v>42</v>
+        <v>95</v>
+      </c>
+      <c r="C51" t="s" s="7">
+        <v>43</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2231,134 +2241,134 @@
     <row r="52" ht="15" customHeight="1">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
-      <c r="C52" t="s" s="8">
-        <v>44</v>
+      <c r="C52" t="s" s="7">
+        <v>45</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
     </row>
     <row r="53" ht="15" customHeight="1">
       <c r="A53" s="2"/>
-      <c r="B53" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="C53" t="s" s="8">
+      <c r="B53" t="s" s="8">
         <v>46</v>
       </c>
-      <c r="D53" t="s" s="9">
+      <c r="C53" t="s" s="7">
         <v>47</v>
+      </c>
+      <c r="D53" t="s" s="8">
+        <v>48</v>
       </c>
       <c r="E53" s="2"/>
     </row>
     <row r="54" ht="15" customHeight="1">
       <c r="A54" s="2"/>
-      <c r="B54" t="s" s="9">
-        <v>48</v>
-      </c>
-      <c r="C54" t="s" s="8">
+      <c r="B54" t="s" s="8">
         <v>49</v>
       </c>
-      <c r="D54" t="s" s="9">
+      <c r="C54" t="s" s="7">
         <v>50</v>
+      </c>
+      <c r="D54" t="s" s="8">
+        <v>51</v>
       </c>
       <c r="E54" s="2"/>
     </row>
     <row r="55" ht="15" customHeight="1">
       <c r="A55" s="2"/>
-      <c r="B55" t="s" s="9">
-        <v>51</v>
-      </c>
-      <c r="C55" t="s" s="8">
+      <c r="B55" t="s" s="8">
         <v>52</v>
       </c>
-      <c r="D55" t="s" s="9">
+      <c r="C55" t="s" s="7">
         <v>53</v>
+      </c>
+      <c r="D55" t="s" s="8">
+        <v>54</v>
       </c>
       <c r="E55" s="2"/>
     </row>
     <row r="56" ht="15" customHeight="1">
       <c r="A56" s="2"/>
-      <c r="B56" t="s" s="9">
-        <v>94</v>
-      </c>
-      <c r="C56" t="s" s="8">
-        <v>55</v>
-      </c>
-      <c r="D56" t="s" s="9">
+      <c r="B56" t="s" s="8">
+        <v>96</v>
+      </c>
+      <c r="C56" t="s" s="7">
         <v>56</v>
+      </c>
+      <c r="D56" t="s" s="8">
+        <v>57</v>
       </c>
       <c r="E56" s="2"/>
     </row>
     <row r="57" ht="15" customHeight="1">
       <c r="A57" s="2"/>
-      <c r="B57" t="s" s="9">
-        <v>95</v>
+      <c r="B57" t="s" s="8">
+        <v>97</v>
       </c>
       <c r="C57" s="2"/>
-      <c r="D57" t="s" s="9">
-        <v>58</v>
+      <c r="D57" t="s" s="8">
+        <v>59</v>
       </c>
       <c r="E57" s="2"/>
     </row>
     <row r="58" ht="15" customHeight="1">
       <c r="A58" s="2"/>
-      <c r="B58" t="s" s="9">
-        <v>96</v>
+      <c r="B58" t="s" s="8">
+        <v>98</v>
       </c>
       <c r="C58" s="2"/>
-      <c r="D58" t="s" s="9">
-        <v>59</v>
+      <c r="D58" t="s" s="8">
+        <v>60</v>
       </c>
       <c r="E58" s="2"/>
     </row>
     <row r="59" ht="15" customHeight="1">
       <c r="A59" s="2"/>
-      <c r="B59" t="s" s="9">
-        <v>97</v>
+      <c r="B59" t="s" s="8">
+        <v>99</v>
       </c>
       <c r="C59" s="2"/>
-      <c r="D59" t="s" s="9">
-        <v>60</v>
+      <c r="D59" t="s" s="8">
+        <v>61</v>
       </c>
       <c r="E59" s="2"/>
     </row>
     <row r="60" ht="15" customHeight="1">
       <c r="A60" s="2"/>
-      <c r="B60" t="s" s="9">
-        <v>98</v>
+      <c r="B60" t="s" s="8">
+        <v>100</v>
       </c>
       <c r="C60" s="2"/>
-      <c r="D60" t="s" s="9">
-        <v>61</v>
+      <c r="D60" t="s" s="8">
+        <v>62</v>
       </c>
       <c r="E60" s="2"/>
     </row>
     <row r="61" ht="15" customHeight="1">
       <c r="A61" s="2"/>
-      <c r="B61" t="s" s="9">
-        <v>99</v>
+      <c r="B61" t="s" s="8">
+        <v>101</v>
       </c>
       <c r="C61" s="2"/>
-      <c r="D61" t="s" s="9">
-        <v>62</v>
+      <c r="D61" t="s" s="8">
+        <v>63</v>
       </c>
       <c r="E61" s="2"/>
     </row>
     <row r="62" ht="15" customHeight="1">
       <c r="A62" s="2"/>
-      <c r="B62" t="s" s="9">
-        <v>54</v>
+      <c r="B62" t="s" s="8">
+        <v>55</v>
       </c>
       <c r="C62" s="2"/>
-      <c r="D62" t="s" s="9">
-        <v>63</v>
+      <c r="D62" t="s" s="8">
+        <v>64</v>
       </c>
       <c r="E62" s="2"/>
     </row>
     <row r="63" ht="15" customHeight="1">
       <c r="A63" s="2"/>
-      <c r="B63" t="s" s="9">
-        <v>57</v>
+      <c r="B63" t="s" s="8">
+        <v>58</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -2381,7 +2391,7 @@
     <row r="66" ht="15" customHeight="1">
       <c r="A66" s="2"/>
       <c r="B66" t="s" s="4">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="5"/>
@@ -2389,7 +2399,7 @@
     </row>
     <row r="67" ht="15" customHeight="1">
       <c r="A67" t="s" s="4">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2399,7 +2409,7 @@
     <row r="68" ht="15" customHeight="1">
       <c r="A68" s="2"/>
       <c r="B68" t="s" s="7">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -2408,7 +2418,7 @@
     <row r="69" ht="15" customHeight="1">
       <c r="A69" s="2"/>
       <c r="B69" t="s" s="7">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -2417,7 +2427,7 @@
     <row r="70" ht="15" customHeight="1">
       <c r="A70" s="2"/>
       <c r="B70" t="s" s="7">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -2426,7 +2436,7 @@
     <row r="71" ht="15" customHeight="1">
       <c r="A71" s="2"/>
       <c r="B71" t="s" s="7">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -2435,7 +2445,7 @@
     <row r="72" ht="15" customHeight="1">
       <c r="A72" s="2"/>
       <c r="B72" t="s" s="7">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -2450,8 +2460,8 @@
     </row>
     <row r="74" ht="15" customHeight="1">
       <c r="A74" s="2"/>
-      <c r="B74" t="s" s="9">
-        <v>57</v>
+      <c r="B74" t="s" s="8">
+        <v>58</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -2481,51 +2491,53 @@
     <row r="78" ht="15" customHeight="1">
       <c r="A78" s="2"/>
       <c r="B78" t="s" s="4">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" t="s" s="4">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E78" s="5"/>
     </row>
     <row r="79" ht="15" customHeight="1">
       <c r="A79" t="s" s="4">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
+      <c r="D79" t="s" s="4">
+        <v>112</v>
+      </c>
       <c r="E79" s="2"/>
     </row>
     <row r="80" ht="15" customHeight="1">
       <c r="A80" t="s" s="4">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B80" t="s" s="7">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="7">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E80" s="2"/>
     </row>
     <row r="81" ht="15" customHeight="1">
       <c r="A81" s="2"/>
       <c r="B81" t="s" s="7">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="7">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E81" s="2"/>
     </row>
     <row r="82" ht="15" customHeight="1">
       <c r="A82" s="2"/>
       <c r="B82" t="s" s="7">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
@@ -2534,22 +2546,22 @@
     <row r="83" ht="15" customHeight="1">
       <c r="A83" s="2"/>
       <c r="B83" t="s" s="7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="7">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E83" s="2"/>
     </row>
     <row r="84" ht="15" customHeight="1">
       <c r="A84" s="2"/>
       <c r="B84" t="s" s="7">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="7">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E84" s="2"/>
     </row>
@@ -2562,12 +2574,12 @@
     </row>
     <row r="86" ht="15" customHeight="1">
       <c r="A86" s="2"/>
-      <c r="B86" t="s" s="9">
-        <v>57</v>
+      <c r="B86" t="s" s="8">
+        <v>58</v>
       </c>
       <c r="C86" s="2"/>
-      <c r="D86" t="s" s="9">
-        <v>47</v>
+      <c r="D86" t="s" s="8">
+        <v>48</v>
       </c>
       <c r="E86" s="2"/>
     </row>
@@ -2575,8 +2587,8 @@
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
-      <c r="D87" t="s" s="9">
-        <v>50</v>
+      <c r="D87" t="s" s="8">
+        <v>51</v>
       </c>
       <c r="E87" s="2"/>
     </row>
@@ -2584,8 +2596,8 @@
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
-      <c r="D88" t="s" s="9">
-        <v>53</v>
+      <c r="D88" t="s" s="8">
+        <v>54</v>
       </c>
       <c r="E88" s="2"/>
     </row>
@@ -2593,8 +2605,8 @@
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
-      <c r="D89" t="s" s="9">
-        <v>56</v>
+      <c r="D89" t="s" s="8">
+        <v>57</v>
       </c>
       <c r="E89" s="2"/>
     </row>
@@ -2602,8 +2614,8 @@
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
-      <c r="D90" t="s" s="9">
-        <v>58</v>
+      <c r="D90" t="s" s="8">
+        <v>59</v>
       </c>
       <c r="E90" s="2"/>
     </row>
@@ -2611,8 +2623,8 @@
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
-      <c r="D91" t="s" s="9">
-        <v>59</v>
+      <c r="D91" t="s" s="8">
+        <v>60</v>
       </c>
       <c r="E91" s="2"/>
     </row>
@@ -2620,8 +2632,8 @@
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
-      <c r="D92" t="s" s="9">
-        <v>60</v>
+      <c r="D92" t="s" s="8">
+        <v>61</v>
       </c>
       <c r="E92" s="2"/>
     </row>
@@ -2629,8 +2641,8 @@
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
-      <c r="D93" t="s" s="9">
-        <v>61</v>
+      <c r="D93" t="s" s="8">
+        <v>62</v>
       </c>
       <c r="E93" s="2"/>
     </row>
@@ -2638,8 +2650,8 @@
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
-      <c r="D94" t="s" s="9">
-        <v>62</v>
+      <c r="D94" t="s" s="8">
+        <v>63</v>
       </c>
       <c r="E94" s="2"/>
     </row>
@@ -2647,8 +2659,8 @@
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-      <c r="D95" t="s" s="9">
-        <v>63</v>
+      <c r="D95" t="s" s="8">
+        <v>64</v>
       </c>
       <c r="E95" s="2"/>
     </row>
@@ -2676,7 +2688,7 @@
     <row r="99" ht="15" customHeight="1">
       <c r="A99" s="2"/>
       <c r="B99" t="s" s="7">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -2684,7 +2696,7 @@
     </row>
     <row r="100" ht="15" customHeight="1">
       <c r="A100" t="s" s="4">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2694,7 +2706,7 @@
     <row r="101" ht="15" customHeight="1">
       <c r="A101" s="2"/>
       <c r="B101" t="s" s="7">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
@@ -2703,7 +2715,7 @@
     <row r="102" ht="15" customHeight="1">
       <c r="A102" s="2"/>
       <c r="B102" t="s" s="7">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
@@ -2712,7 +2724,7 @@
     <row r="103" ht="15" customHeight="1">
       <c r="A103" s="2"/>
       <c r="B103" t="s" s="7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
@@ -2721,7 +2733,7 @@
     <row r="104" ht="15" customHeight="1">
       <c r="A104" s="2"/>
       <c r="B104" t="s" s="7">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -2736,8 +2748,8 @@
     </row>
     <row r="106" ht="15" customHeight="1">
       <c r="A106" s="2"/>
-      <c r="B106" t="s" s="9">
-        <v>57</v>
+      <c r="B106" t="s" s="8">
+        <v>58</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -2753,6 +2765,101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="8.85156" style="9" customWidth="1"/>
+    <col min="2" max="2" width="8.85156" style="9" customWidth="1"/>
+    <col min="3" max="3" width="8.85156" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="9" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="9" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="25" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -2845,99 +2952,4 @@
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="8.85156" style="11" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="11" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="11" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="11" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="11" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="25" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>